<commit_message>
--intermediate commit due to laptop issues so I can push to GitHub private repos to work on a different computer--
</commit_message>
<xml_diff>
--- a/docs/auth_app_recs.xlsx
+++ b/docs/auth_app_recs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>APP_GROUP_NAME</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>benjamin.richards</t>
+  </si>
+  <si>
+    <t>kyle.koyanagi</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,6 +548,18 @@
         <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('benjamin.richards', '', 'Y');</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" ref="D8" si="2">CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ") VALUES ('", A8, "', '", SUBSTITUTE(B8, "'", "''"), "', '", C8, "');")</f>
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('kyle.koyanagi', '', 'Y');</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -553,10 +568,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,6 +663,18 @@
         <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'benjamin.richards'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" ref="C8" si="2">CONCATENATE("INSERT INTO AUTH_APP_USER_GROUPS (",A$1, ", ", B$1, ") VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = '", A8, "'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = '", SUBSTITUTE(B8, "'", "''"), "'));")</f>
+        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'kyle.koyanagi'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
updated user group data and grant_info.sql for the APEX application
</commit_message>
<xml_diff>
--- a/docs/auth_app_recs.xlsx
+++ b/docs/auth_app_recs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="48">
   <si>
     <t>APP_GROUP_NAME</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Y</t>
   </si>
   <si>
+    <t>noriko.shoji</t>
+  </si>
+  <si>
     <t>APP_USER_ID</t>
   </si>
   <si>
@@ -65,7 +68,49 @@
     <t>DATA_ADMIN</t>
   </si>
   <si>
-    <t>noriko.shoji</t>
+    <t>APP_USER_FIRST_NAME</t>
+  </si>
+  <si>
+    <t>APP_USER_LAST_NAME</t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>Abdul</t>
+  </si>
+  <si>
+    <t>Nori</t>
+  </si>
+  <si>
+    <t>Shoji</t>
+  </si>
+  <si>
+    <t>leonora.fukuda</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Fukuda</t>
+  </si>
+  <si>
+    <t>PIFSC.ITS.TEST</t>
+  </si>
+  <si>
+    <t>ITS</t>
+  </si>
+  <si>
+    <t>Testing Account</t>
+  </si>
+  <si>
+    <t>DATA_WRITE</t>
+  </si>
+  <si>
+    <t>Read/Write</t>
+  </si>
+  <si>
+    <t>Read/Write users that can perform database actions</t>
   </si>
   <si>
     <t>chad.yoshinaga</t>
@@ -81,6 +126,45 @@
   </si>
   <si>
     <t>kyle.koyanagi</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Yoshinaga</t>
+  </si>
+  <si>
+    <t>Russell</t>
+  </si>
+  <si>
+    <t>Reardon</t>
+  </si>
+  <si>
+    <t>Kristin</t>
+  </si>
+  <si>
+    <t>Sojka</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Richards</t>
+  </si>
+  <si>
+    <t>Kyle</t>
+  </si>
+  <si>
+    <t>Koyanagi</t>
+  </si>
+  <si>
+    <t>Frank.Parish</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Parish</t>
   </si>
 </sst>
 </file>
@@ -398,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +515,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -439,6 +523,21 @@
       <c r="D2" t="str">
         <f>CONCATENATE("INSERT INTO AUTH_APP_GROUPS (",A$1, ", ", B$1, ", ", C$1, ") VALUES ('", A2, "', '", SUBSTITUTE(B2, "'", "''"), "', '", C2, "');")</f>
         <v>INSERT INTO AUTH_APP_GROUPS (APP_GROUP_NAME, APP_GROUP_CODE, APP_GROUP_DESC) VALUES ('Administrators', 'DATA_ADMIN', 'Administrative users that can edit data for any division/program');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="str">
+        <f>CONCATENATE("INSERT INTO AUTH_APP_GROUPS (",A$1, ", ", B$1, ", ", C$1, ") VALUES ('", A3, "', '", SUBSTITUTE(B3, "'", "''"), "', '", C3, "');")</f>
+        <v>INSERT INTO AUTH_APP_GROUPS (APP_GROUP_NAME, APP_GROUP_CODE, APP_GROUP_DESC) VALUES ('Read/Write', 'DATA_WRITE', 'Read/Write users that can perform database actions');</v>
       </c>
     </row>
   </sheetData>
@@ -449,115 +548,218 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="str">
-        <f>CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ") VALUES ('", A2, "', '", SUBSTITUTE(B2, "'", "''"), "', '", C2, "');")</f>
-        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('jesse.abdul', '', 'Y');</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="str">
+        <f>CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ") VALUES ('", A2, "', '", SUBSTITUTE(B2, "'", "''"), "', '", SUBSTITUTE(C2, "'", "''"), "', '", SUBSTITUTE(D2, "'", "''"), "', '", E2, "');")</f>
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('jesse.abdul', 'Jesse', 'Abdul', '', 'Y');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
       </c>
       <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D5" si="0">CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ") VALUES ('", A3, "', '", SUBSTITUTE(B3, "'", "''"), "', '", C3, "');")</f>
-        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('noriko.shoji', '', 'Y');</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F4" si="0">CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ") VALUES ('", A3, "', '", SUBSTITUTE(B3, "'", "''"), "', '", SUBSTITUTE(C3, "'", "''"), "', '", SUBSTITUTE(D3, "'", "''"), "', '", E3, "');")</f>
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('noriko.shoji', 'Nori', 'Shoji', '', 'Y');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
       </c>
       <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="str">
+      <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('chad.yoshinaga', '', 'Y');</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('leonora.fukuda', 'Leo', 'Fukuda', '', 'Y');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
       </c>
       <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('russell.reardon', '', 'Y');</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F9" si="1">CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ") VALUES ('", A5, "', '", SUBSTITUTE(B5, "'", "''"), "', '", SUBSTITUTE(C5, "'", "''"), "', '", SUBSTITUTE(D5, "'", "''"), "', '", E5, "');")</f>
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('chad.yoshinaga', 'Chad', 'Yoshinaga', '', 'Y');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
       </c>
       <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="str">
-        <f t="shared" ref="D6:D7" si="1">CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ") VALUES ('", A6, "', '", SUBSTITUTE(B6, "'", "''"), "', '", C6, "');")</f>
-        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('kristin.m.sojka', '', 'Y');</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('russell.reardon', 'Russell', 'Reardon', '', 'Y');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
       </c>
       <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="str">
+      <c r="F7" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('benjamin.richards', '', 'Y');</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('kristin.m.sojka', 'Kristin', 'Sojka', '', 'Y');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
       </c>
       <c r="C8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" t="str">
-        <f t="shared" ref="D8" si="2">CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ") VALUES ('", A8, "', '", SUBSTITUTE(B8, "'", "''"), "', '", C8, "');")</f>
-        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('kyle.koyanagi', '', 'Y');</v>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('benjamin.richards', 'Benjamin', 'Richards', '', 'Y');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('kyle.koyanagi', 'Kyle', 'Koyanagi', '', 'Y');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="str">
+        <f>CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ") VALUES ('", A10, "', '", SUBSTITUTE(B10, "'", "''"), "', '", SUBSTITUTE(C10, "'", "''"), "', '", SUBSTITUTE(D10, "'", "''"), "', '", E10, "');")</f>
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('PIFSC.ITS.TEST', 'ITS', 'Testing Account', '', 'Y');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="str">
+        <f>CONCATENATE("INSERT INTO AUTH_APP_USERS (",A$1, ", ", B$1, ", ", C$1, ", ", D$1, ", ", E$1, ") VALUES ('", A11, "', '", SUBSTITUTE(B11, "'", "''"), "', '", SUBSTITUTE(C11, "'", "''"), "', '", SUBSTITUTE(D11, "'", "''"), "', '", E11, "');")</f>
+        <v>INSERT INTO AUTH_APP_USERS (APP_USER_NAME, APP_USER_FIRST_NAME, APP_USER_LAST_NAME, APP_USER_COMMENTS, APP_USER_ACTIVE_YN) VALUES ('Frank.Parish', 'Frank', 'Parish', '', 'Y');</v>
       </c>
     </row>
   </sheetData>
@@ -568,10 +770,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C11" sqref="C2:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,10 +784,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -596,7 +798,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE("INSERT INTO AUTH_APP_USER_GROUPS (",A$1, ", ", B$1, ") VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = '", A2, "'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = '", SUBSTITUTE(B2, "'", "''"), "'));")</f>
@@ -605,74 +807,110 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C5" si="0">CONCATENATE("INSERT INTO AUTH_APP_USER_GROUPS (",A$1, ", ", B$1, ") VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = '", A3, "'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = '", SUBSTITUTE(B3, "'", "''"), "'));")</f>
+        <f t="shared" ref="C3:C11" si="0">CONCATENATE("INSERT INTO AUTH_APP_USER_GROUPS (",A$1, ", ", B$1, ") VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = '", A3, "'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = '", SUBSTITUTE(B3, "'", "''"), "'));")</f>
         <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'noriko.shoji'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'chad.yoshinaga'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
+        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'leonora.fukuda'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'russell.reardon'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
+        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'chad.yoshinaga'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" ref="C6:C7" si="1">CONCATENATE("INSERT INTO AUTH_APP_USER_GROUPS (",A$1, ", ", B$1, ") VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = '", A6, "'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = '", SUBSTITUTE(B6, "'", "''"), "'));")</f>
-        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'kristin.m.sojka'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'russell.reardon'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="1"/>
-        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'benjamin.richards'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'kristin.m.sojka'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" ref="C8" si="2">CONCATENATE("INSERT INTO AUTH_APP_USER_GROUPS (",A$1, ", ", B$1, ") VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = '", A8, "'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = '", SUBSTITUTE(B8, "'", "''"), "'));")</f>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'benjamin.richards'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
         <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'kyle.koyanagi'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'PIFSC.ITS.TEST'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO AUTH_APP_USER_GROUPS (APP_USER_ID, APP_GROUP_ID) VALUES ((SELECT APP_USER_ID FROM AUTH_APP_USERS WHERE APP_USER_NAME = 'Frank.Parish'), (SELECT APP_GROUP_ID FROM AUTH_APP_GROUPS WHERE APP_GROUP_CODE = 'DATA_ADMIN'));</v>
       </c>
     </row>
   </sheetData>

</xml_diff>